<commit_message>
Re named all bot versions.
Re named and gave adjustments to all of the released versions of Mybot. The version increases are now consistent, lots have been deleted and the latest version is now called v2.4
</commit_message>
<xml_diff>
--- a/MyChessBots.xlsx
+++ b/MyChessBots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://templestowecvicedu-my.sharepoint.com/personal/ric0016_tc_vic_edu_au/Documents/Desktop/Documents/GitHub/Rohan_Chess_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{71E6F730-4C8B-4834-B52F-814EDD5A6C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A0AD038-9B47-4B55-91D1-C2730FC9F2C3}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="13_ncr:1_{71E6F730-4C8B-4834-B52F-814EDD5A6C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5769302C-8A84-4551-8F5A-80A2A5E41F96}"/>
   <bookViews>
-    <workbookView xWindow="2712" yWindow="1944" windowWidth="17280" windowHeight="8880" xr2:uid="{32A029A6-4FBE-439A-A203-1D064A31895A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" xr2:uid="{32A029A6-4FBE-439A-A203-1D064A31895A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Versions:</t>
   </si>
@@ -50,31 +50,13 @@
     <t>Read first:</t>
   </si>
   <si>
-    <t>1.5.1</t>
-  </si>
-  <si>
     <t>D3: (500)*2 or 1000 Games</t>
-  </si>
-  <si>
-    <t>2.3*</t>
   </si>
   <si>
     <t>*Depth now starts at 4 for first 5 seconds</t>
   </si>
   <si>
-    <t>2.5.1</t>
-  </si>
-  <si>
-    <t>2.5.1 Fast</t>
-  </si>
-  <si>
     <t>Fast means that depth is just 3</t>
-  </si>
-  <si>
-    <t>2.6.1</t>
-  </si>
-  <si>
-    <t>2.6.2</t>
   </si>
 </sst>
 </file>
@@ -116,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -125,11 +107,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -162,6 +152,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D42F3CF-5A9F-4664-9D92-4BFF33076767}">
   <dimension ref="A1:AF46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O18" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AD30" sqref="AD30"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,15 +487,15 @@
     <col min="2" max="2" width="18.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,53 +544,35 @@
       <c r="Q2" s="1">
         <v>1.5</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>4</v>
+      <c r="R2" s="1">
+        <v>1.6</v>
       </c>
       <c r="S2" s="1">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="T2" s="1">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="U2" s="1">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="V2" s="1">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="W2" s="1">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="X2" s="1">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Y2" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA2" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Z2" s="1">
         <v>2.4</v>
       </c>
-      <c r="AB2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -604,12 +580,12 @@
         <v>0.1</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="R3">
+      <c r="N3">
         <f>(0-495)*2</f>
         <v>-990</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -617,100 +593,96 @@
         <v>0.2</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="R4">
+      <c r="N4">
         <f>(0-499)*2</f>
         <v>-998</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>0.3</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="R5">
+      <c r="N5">
         <f>(0-490)*2</f>
         <v>-980</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>0.4</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="R6">
+      <c r="N6">
         <f>28-490</f>
         <v>-462</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>0.5</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="R7">
-        <f>(19-233)*2</f>
-        <v>-428</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="N7">
+        <f>359-567</f>
+        <v>-208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>0.6</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="R8">
-        <f>19-540</f>
-        <v>-521</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>0.7</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="R9">
-        <f>359-567</f>
-        <v>-208</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>0.8</v>
       </c>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>0.9</v>
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>1.2</v>
       </c>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>1.3</v>
       </c>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>1.4</v>
+      </c>
+      <c r="N16">
+        <f>428-482</f>
+        <v>-54</v>
       </c>
       <c r="P16" s="2"/>
     </row>
@@ -718,166 +690,116 @@
       <c r="B17" s="1">
         <v>1.5</v>
       </c>
+      <c r="N17">
+        <f>(252-206)*2</f>
+        <v>92</v>
+      </c>
       <c r="Q17" s="2"/>
     </row>
     <row r="18" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
-        <v>4</v>
+      <c r="B18" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="N18">
+        <f>514-403</f>
+        <v>111</v>
       </c>
       <c r="R18" s="2"/>
     </row>
     <row r="19" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="S19" s="2"/>
     </row>
     <row r="20" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="T20" s="2"/>
     </row>
     <row r="21" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="R21">
-        <f>428-482</f>
-        <v>-54</v>
+        <v>1.9</v>
+      </c>
+      <c r="N21">
+        <f>(269-193)*2</f>
+        <v>152</v>
       </c>
       <c r="U21" s="2"/>
     </row>
     <row r="22" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
-        <v>1.9</v>
-      </c>
-      <c r="R22">
-        <f>428-482</f>
-        <v>-54</v>
+        <v>2</v>
       </c>
       <c r="V22" s="2"/>
     </row>
     <row r="23" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
-        <v>2</v>
-      </c>
-      <c r="R23">
-        <f>(252-206)*2</f>
-        <v>92</v>
+        <v>2.1</v>
       </c>
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="R24">
-        <f>514-403</f>
-        <v>111</v>
-      </c>
-      <c r="W24">
-        <f>(251-213)*2</f>
-        <v>76</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="X24" s="2"/>
     </row>
     <row r="25" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="R25">
-        <f>(258-204)*2</f>
-        <v>108</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="Y25" s="2"/>
     </row>
     <row r="26" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R26">
-        <f>815-124</f>
-        <v>691</v>
+      <c r="B26" s="1">
+        <v>2.4</v>
       </c>
       <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B27" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="R27">
-        <f>855-79</f>
-        <v>776</v>
-      </c>
-      <c r="Z27">
-        <f>(200-127)*2</f>
-        <v>146</v>
-      </c>
-      <c r="AA27" s="2"/>
+      <c r="AA27" s="4"/>
     </row>
     <row r="28" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB28" s="2"/>
+      <c r="AB28" s="4"/>
     </row>
     <row r="29" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R29">
-        <f>(269-193)*2</f>
-        <v>152</v>
-      </c>
-      <c r="AC29" s="2"/>
+      <c r="AC29" s="4"/>
     </row>
     <row r="30" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B30" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="AD30" s="2"/>
+      <c r="AD30" s="4"/>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE31" s="2"/>
+      <c r="AE31" s="4"/>
     </row>
     <row r="32" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE32">
-        <f>(422-407)</f>
-        <v>15</v>
-      </c>
-      <c r="AF32" s="2"/>
+      <c r="AF32" s="4"/>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:DB732">
+  <conditionalFormatting sqref="C9:Q9 S9:DB9 C8:DB8 S3:DB7 C3:Q7 C35:DB732 S21:DB34 C30:Q34 C10:DB20 N27 C22:M29 O22:Q29 C21:Q21">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="num" val="-750"/>
+        <cfvo type="num" val="-650"/>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="750"/>
+        <cfvo type="num" val="650"/>
         <color rgb="FFA20000"/>
         <color rgb="FFFFFF3B"/>
         <color rgb="FF0F9325"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:U16 C3:Q17 T17:U17 S18 T19:U19 C19:Q21 S20:U21">
+  <conditionalFormatting sqref="S3:U16 T17:U17 S18 T19:U19 S20:U21 C19:Q20 C21:M21 O21:Q21 C3:Q17">
     <cfRule type="cellIs" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
MYBOT V3 AND A WHOLE LOT OF VERSIONS
MYBOT3 v0.4 and onwards are finally stronger than 3.4.1
</commit_message>
<xml_diff>
--- a/MyChessBots.xlsx
+++ b/MyChessBots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\GitHub\Rohan_Chess_Bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://templestowecvicedu-my.sharepoint.com/personal/ric0016_tc_vic_edu_au/Documents/Desktop/Coding/Rohan_Chess_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CAB578-ED10-431A-9D22-5C1DBF858A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{47CAB578-ED10-431A-9D22-5C1DBF858A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A248AC5-5028-49AB-BCC2-425E98C5A0AE}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="3336" windowWidth="23040" windowHeight="12120" xr2:uid="{32A029A6-4FBE-439A-A203-1D064A31895A}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="21164" windowHeight="11291" xr2:uid="{32A029A6-4FBE-439A-A203-1D064A31895A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>Versions:</t>
   </si>
@@ -111,6 +111,39 @@
   </si>
   <si>
     <t>2 v0.5 depth compare Q depth = infinite</t>
+  </si>
+  <si>
+    <t>trustbot1.0</t>
+  </si>
+  <si>
+    <t>mybot(2) v3.4.1</t>
+  </si>
+  <si>
+    <t>125games</t>
+  </si>
+  <si>
+    <t>d7</t>
+  </si>
+  <si>
+    <t>d8</t>
+  </si>
+  <si>
+    <t>New D5 battles:</t>
+  </si>
+  <si>
+    <t>3.4.1</t>
+  </si>
+  <si>
+    <t>5s+40ms</t>
+  </si>
+  <si>
+    <t>Sample size</t>
+  </si>
+  <si>
+    <t>5+0.05s</t>
+  </si>
+  <si>
+    <t>tied</t>
   </si>
 </sst>
 </file>
@@ -307,6 +340,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -626,20 +663,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D42F3CF-5A9F-4664-9D92-4BFF33076767}">
-  <dimension ref="A1:AA46"/>
+  <dimension ref="A1:AA74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="75" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="133" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.796875" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="10" max="10" width="25.77734375" customWidth="1"/>
+    <col min="10" max="10" width="25.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
@@ -1085,7 +1123,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="14.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -1110,7 +1148,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="15.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -1135,17 +1173,244 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:12" ht="14.75" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B45" s="3"/>
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="3">
+        <f>14-95</f>
+        <v>-81</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B46" s="3"/>
+      <c r="A46">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B46" s="3">
+        <f>25-74</f>
+        <v>-49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1.2</v>
+      </c>
+      <c r="B47" s="1">
+        <f>32-77</f>
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1.3</v>
+      </c>
+      <c r="B48" s="1">
+        <f>33-76</f>
+        <v>-43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1.4</v>
+      </c>
+      <c r="B49" s="1">
+        <f>(56+16)/182</f>
+        <v>0.39560439560439559</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>1.5</v>
+      </c>
+      <c r="B50" s="1">
+        <f>(73+12)/216</f>
+        <v>0.39351851851851855</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1.6</v>
+      </c>
+      <c r="B51" s="1">
+        <f>(85+14)/201</f>
+        <v>0.4925373134328358</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>1.7</v>
+      </c>
+      <c r="B52" s="1">
+        <f>(87+19)/206</f>
+        <v>0.5145631067961165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>1.8</v>
+      </c>
+      <c r="B53" s="1">
+        <f>(222+95/2)/560</f>
+        <v>0.48125000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>1.9</v>
+      </c>
+      <c r="B54" s="1">
+        <f>(397+93)/1000</f>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>2.1</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>1.8</v>
+      </c>
+      <c r="B65" s="1">
+        <f>(315+157/2)/755</f>
+        <v>0.52119205298013249</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D67" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>2.1</v>
+      </c>
+      <c r="B68" s="1">
+        <f>(112+22)/252</f>
+        <v>0.53174603174603174</v>
+      </c>
+      <c r="C68" s="1">
+        <f>(95+25)/312</f>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="D68">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>0.1</v>
+      </c>
+      <c r="C69">
+        <f>(117+32)/329</f>
+        <v>0.45288753799392095</v>
+      </c>
+      <c r="D69">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>0.2</v>
+      </c>
+      <c r="C70">
+        <f>(101+24)/250</f>
+        <v>0.5</v>
+      </c>
+      <c r="D70">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>0.3</v>
+      </c>
+      <c r="C71">
+        <f>(159+30)/369</f>
+        <v>0.51219512195121952</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>0.4</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C9:Q9 S9:DB9 C8:DB8 S3:DB7 C3:Q7 C30:Q31 C10:DB20 N27 C22:M29 O22:Q29 C21:Q21 C40:DB732 S21:DB34 M32:Q34 M35:DB39">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="C32:E39 H32:I39 L32:L39">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="-650"/>
         <cfvo type="num" val="0"/>
@@ -1156,8 +1421,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32:E39 H32:I39 L32:L39">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="C9:Q9 S9:DB9 C8:DB8 S3:DB7 C3:Q7 C30:Q31 C10:DB20 N27 C22:M29 O22:Q29 C21:Q21 C40:DB67 S21:DB34 M32:Q34 M35:DB39 C154:DB732 C118:C153 E68:DB153">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="-650"/>
         <cfvo type="num" val="0"/>
@@ -1193,5 +1458,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>